<commit_message>
vault backup: 2024-12-03 14:03:12
</commit_message>
<xml_diff>
--- a/FP/공유모빌리티FP.xlsx
+++ b/FP/공유모빌리티FP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이준한\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GreatBPS\Pusan\FP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BC53813-F3FE-47DB-A834-C8073621CD8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29BD63F-0265-4E52-8F47-99FBFAEF7378}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13095" xr2:uid="{53CE6B40-7889-4B9B-B108-70B5FC90B0A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>수정된 FP 및 단위 기능</t>
   </si>
@@ -138,9 +138,6 @@
     <t>EIF: 대중교통 API (5)</t>
   </si>
   <si>
-    <t>- 할인 계산 및 적용</t>
-  </si>
-  <si>
     <t>- 할인 내역 저장</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
   </si>
   <si>
     <t>ILF: 관리자 데이터 (7)</t>
-  </si>
-  <si>
-    <t>변경 후 FP 요약</t>
   </si>
   <si>
     <r>
@@ -222,12 +216,137 @@
       <t>로 조정되었습니다. 할인 기능은 사용자에게 부가적인 편의성을 제공하며, 대여 서비스와 대중교통 연계의 가치를 높이는 중요한 요소로 작용합니다.</t>
     </r>
   </si>
+  <si>
+    <t>설명</t>
+  </si>
+  <si>
+    <t>회원 정보를 입력받아 등록하고 저장</t>
+  </si>
+  <si>
+    <t>사용자의 인증 정보를 확인하고 세션을 생성</t>
+  </si>
+  <si>
+    <t>사용자 정보와 선호 설정을 저장</t>
+  </si>
+  <si>
+    <t>사용자가 대여를 시작할 수 있도록 요청 처리</t>
+  </si>
+  <si>
+    <t>사용자가 대여 종료 및 반납 요청을 처리</t>
+  </si>
+  <si>
+    <t>사용자의 위치 기반으로 대여 가능한 기기를 조회</t>
+  </si>
+  <si>
+    <t>대여 및 반납 이력을 기록하고 저장</t>
+  </si>
+  <si>
+    <t>결제 금액과 세부 정보를 확인하고 결제를 요청</t>
+  </si>
+  <si>
+    <t>결제가 완료되면 확인 후 영수증을 발행</t>
+  </si>
+  <si>
+    <t>PG사와 데이터 교환을 통해 결제를 처리</t>
+  </si>
+  <si>
+    <t>사용자가 원하는 기기 예약 요청을 처리</t>
+  </si>
+  <si>
+    <t>사용자의 요청에 따라 기존 예약을 취소</t>
+  </si>
+  <si>
+    <t>예약 내역을 기록하고 저장</t>
+  </si>
+  <si>
+    <t>GPS 데이터를 기반으로 기기의 현재 위치를 조회</t>
+  </si>
+  <si>
+    <t>외부 GPS 서비스와의 연계를 통해 위치 데이터를 제공</t>
+  </si>
+  <si>
+    <t>외부 API를 통해 사용자의 대중교통 이용 내역을 확인</t>
+  </si>
+  <si>
+    <t>- 할인 조건 확인</t>
+  </si>
+  <si>
+    <t>대중교통 이용 여부와 할인 조건을 확인</t>
+  </si>
+  <si>
+    <t>- 할인 금액 계산</t>
+  </si>
+  <si>
+    <t>대중교통 이용 내역에 따라 할인 금액을 계산</t>
+  </si>
+  <si>
+    <t>- 할인 금액 적용</t>
+  </si>
+  <si>
+    <t>계산된 할인 금액을 최종 결제에 반영</t>
+  </si>
+  <si>
+    <t>할인 내역을 기록하고 저장</t>
+  </si>
+  <si>
+    <t>사용자, 대여, 결제 데이터를 추가, 수정, 삭제</t>
+  </si>
+  <si>
+    <t>대여 및 결제 데이터에 대한 통계 보고서를 생성</t>
+  </si>
+  <si>
+    <t>관리자 계정 정보와 권한 정보를 저장</t>
+  </si>
+  <si>
+    <r>
+      <t>총 FP: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.75"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>85</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>이 표는 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>단위 기능 설명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>을 포함해 각 기능이 수행하는 역할과 관련 데이터를 명확히 나타냅니다.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,14 +357,6 @@
     </font>
     <font>
       <sz val="13.75"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.6"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -290,6 +401,30 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.75"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -299,7 +434,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -362,17 +497,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -385,7 +509,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -395,38 +519,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,6 +573,10 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
@@ -474,7 +605,57 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{515892B2-D4DB-4583-92C9-D86F6C69843A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>50</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Control 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51134835-804B-4F8C-BA1C-A47B0D3CD6DF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -802,10 +983,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39A3D2D-455A-4EC1-81A5-EB1F506B9512}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:F63"/>
+  <dimension ref="C3:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -815,493 +996,546 @@
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="87" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" ht="87" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10" t="s">
+    <row r="5" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="12"/>
-      <c r="D7" s="6" t="s">
+    <row r="7" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="6"/>
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="12"/>
-      <c r="D8" s="6" t="s">
+    <row r="8" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="6"/>
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="12"/>
-      <c r="D9" s="5" t="s">
+    <row r="9" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="6"/>
+      <c r="D9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="11" t="s">
+    <row r="10" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="12"/>
-      <c r="D11" s="6" t="s">
+    <row r="11" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="6"/>
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:6" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="12"/>
-      <c r="D12" s="6" t="s">
+    <row r="12" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="6"/>
+      <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="7">
+      <c r="G12" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="12"/>
-      <c r="D13" s="6" t="s">
+    <row r="13" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="6"/>
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="7">
+      <c r="G13" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="12"/>
-      <c r="D14" s="5" t="s">
+    <row r="14" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="6"/>
+      <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="11">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="11" t="s">
+    <row r="15" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="12"/>
-      <c r="D16" s="6" t="s">
+    <row r="16" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="6"/>
+      <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="12"/>
-      <c r="D17" s="6" t="s">
+    <row r="17" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="6"/>
+      <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="7">
+      <c r="G17" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="12"/>
-      <c r="D18" s="5" t="s">
+    <row r="18" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="6"/>
+      <c r="D18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="11">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="11" t="s">
+    <row r="19" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="7">
+      <c r="G19" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="12"/>
-      <c r="D20" s="6" t="s">
+    <row r="20" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="6"/>
+      <c r="D20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="7">
+      <c r="G20" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="12"/>
-      <c r="D21" s="6" t="s">
+    <row r="21" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="6"/>
+      <c r="D21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="12"/>
-      <c r="D22" s="5" t="s">
+    <row r="22" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="6"/>
+      <c r="D22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="8">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="11" t="s">
+    <row r="23" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="7">
+      <c r="G23" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="12"/>
-      <c r="D24" s="6" t="s">
+    <row r="24" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="6"/>
+      <c r="D24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="7">
+      <c r="G24" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="12"/>
-      <c r="D25" s="5" t="s">
+    <row r="25" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="6"/>
+      <c r="D25" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="11" t="s">
+    <row r="26" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="7">
+      <c r="G26" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="12"/>
-      <c r="D27" s="6" t="s">
+    <row r="27" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="6"/>
+      <c r="D27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="6"/>
+      <c r="D28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="6"/>
+      <c r="D29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="6"/>
+      <c r="D30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="6"/>
+      <c r="D31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="6"/>
+      <c r="D33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="7">
+      <c r="G33" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="3:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="12"/>
-      <c r="D28" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="7">
+    <row r="34" spans="3:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="6"/>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="12"/>
-      <c r="D29" s="5" t="s">
+    <row r="35" spans="3:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="6"/>
+      <c r="D35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="8">
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="11">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="12"/>
-      <c r="D31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="12"/>
-      <c r="D32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="6" t="s">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="3:7" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="C43" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="3:3" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="C49" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="7"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="3:3" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="C58" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="12"/>
-      <c r="D33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:6" ht="65.25" x14ac:dyDescent="0.3">
-      <c r="C41" s="2" t="s">
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="3:3" ht="396" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C53" s="1"/>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="3:4" ht="43.5" x14ac:dyDescent="0.3">
-      <c r="C58" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="3:4" ht="396" x14ac:dyDescent="0.3">
-      <c r="C60" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C61" s="13"/>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C63" s="13"/>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="7"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C63" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1309,7 +1543,32 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>50</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>51</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -1329,7 +1588,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>